<commit_message>
-Created the definition for the MyInteger Class. -Updated the Excel document to include a UML diagram for this class.
</commit_message>
<xml_diff>
--- a/UML Diagrams.xlsx
+++ b/UML Diagrams.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmorledge-hampton19\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\Source\Repos\CS172-Homework-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Fan</t>
   </si>
@@ -114,14 +114,158 @@
   </si>
   <si>
     <t xml:space="preserve"> +getPrevious(): int</t>
+  </si>
+  <si>
+    <t>My Integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +MyInteger(newValue: int)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +getValue():  int const</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + isEven(): bool const</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +isOdd(): bool const</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +isPrime(): bool const</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+isEven(checkThis: int): bool</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+isOdd(checkThis: int): bool</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+isEven(checkThis: MyInteger&amp; const): bool</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+isOdd(checkThis: MyInteger&amp; const): bool</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+isPrime(checkThis: MyInteger&amp; const): bool</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+isPrime(checkThis: int): bool</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> +equals(checkThis: int): bool const</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +equals(checkThis: MyInteger&amp; const): bool const</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+parseInt(parseThis: string&amp; const): int</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -504,20 +648,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="55.28515625" customWidth="1"/>
-    <col min="3" max="3" width="54.85546875" customWidth="1"/>
-    <col min="5" max="5" width="44.140625" customWidth="1"/>
+    <col min="1" max="1" width="55.265625" customWidth="1"/>
+    <col min="3" max="3" width="54.86328125" customWidth="1"/>
+    <col min="5" max="5" width="44.1328125" customWidth="1"/>
+    <col min="7" max="7" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -527,8 +672,11 @@
       <c r="E1" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -539,8 +687,11 @@
       <c r="E2" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -551,8 +702,11 @@
       <c r="E3" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -562,8 +716,11 @@
       <c r="E4" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -573,8 +730,11 @@
       <c r="E5" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -584,8 +744,11 @@
       <c r="E6" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -595,8 +758,11 @@
       <c r="E7" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -604,8 +770,11 @@
         <v>19</v>
       </c>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -613,8 +782,11 @@
         <v>20</v>
       </c>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -622,8 +794,11 @@
         <v>21</v>
       </c>
       <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -631,79 +806,105 @@
         <v>22</v>
       </c>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G14" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G15" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G16" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="1"/>
     </row>
   </sheetData>

</xml_diff>